<commit_message>
fotos gic, correcciones main informe
</commit_message>
<xml_diff>
--- a/Ej1/Mediciones/tc_tp3_ej1_hf.xlsx
+++ b/Ej1/Mediciones/tc_tp3_ej1_hf.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>f</t>
   </si>
@@ -32,11 +32,14 @@
   <si>
     <t>modH</t>
   </si>
+  <si>
+    <t>dV/dt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -79,14 +82,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -98,7 +104,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -281,6 +286,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-849A-4325-A527-56F5B0D54F2F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -328,7 +338,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -344,9 +353,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -358,7 +367,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -541,6 +549,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-95A8-4583-8196-B92802893D1E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -588,7 +601,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -620,7 +632,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="1 Gráfico"/>
+        <xdr:cNvPr id="2" name="1 Gráfico">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -650,7 +668,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="2 Gráfico"/>
+        <xdr:cNvPr id="3" name="2 Gráfico">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -669,7 +693,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -711,7 +735,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -744,9 +768,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -779,6 +820,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -955,18 +1013,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -982,8 +1040,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.01</v>
       </c>
@@ -997,11 +1058,15 @@
         <v>89</v>
       </c>
       <c r="E2">
-        <f>20*LOG10(C2/B2)</f>
+        <f t="shared" ref="E2:E13" si="0">20*LOG10(C2/B2)</f>
         <v>-51.867476242857393</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1">
+        <f>C2*A2*1000/10^6</f>
+        <v>5.0500000000000004E-7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.02</v>
       </c>
@@ -1015,11 +1080,15 @@
         <v>90</v>
       </c>
       <c r="E3">
-        <f>20*LOG10(C3/B3)</f>
+        <f t="shared" si="0"/>
         <v>-45.846876329577775</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F25" si="1">C3*A3*1000/10^6</f>
+        <v>2.0200000000000001E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.05</v>
       </c>
@@ -1033,11 +1102,15 @@
         <v>89</v>
       </c>
       <c r="E4">
-        <f>20*LOG10(C4/B4)</f>
+        <f t="shared" si="0"/>
         <v>-37.905292989599737</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
+        <v>1.26E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.1</v>
       </c>
@@ -1051,11 +1124,15 @@
         <v>89</v>
       </c>
       <c r="E5">
-        <f>20*LOG10(C5/B5)</f>
+        <f t="shared" si="0"/>
         <v>-31.953903718510247</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.2</v>
       </c>
@@ -1069,11 +1146,15 @@
         <v>88</v>
       </c>
       <c r="E6">
-        <f>20*LOG10(C6/B6)</f>
+        <f t="shared" si="0"/>
         <v>-25.846876329577771</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>2.02E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -1087,11 +1168,15 @@
         <v>86</v>
       </c>
       <c r="E7">
-        <f>20*LOG10(C7/B7)</f>
+        <f t="shared" si="0"/>
         <v>-17.435671072609281</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>1.33E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1105,11 +1190,15 @@
         <v>80</v>
       </c>
       <c r="E8">
-        <f>20*LOG10(C8/B8)</f>
+        <f t="shared" si="0"/>
         <v>-9.4377745557197095</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>6.6800000000000002E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1.5</v>
       </c>
@@ -1123,11 +1212,15 @@
         <v>65</v>
       </c>
       <c r="E9">
-        <f>20*LOG10(C9/B9)</f>
+        <f t="shared" si="0"/>
         <v>-1.6320144034207558</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
+        <v>1.3424999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1.8</v>
       </c>
@@ -1141,11 +1234,15 @@
         <v>34</v>
       </c>
       <c r="E10">
-        <f>20*LOG10(C10/B10)</f>
+        <f t="shared" si="0"/>
         <v>4.1922858639868945</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>3.15E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1.94</v>
       </c>
@@ -1159,11 +1256,15 @@
         <v>5</v>
       </c>
       <c r="E11">
-        <f>20*LOG10(C11/B11)</f>
+        <f t="shared" si="0"/>
         <v>5.6286887920120101</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>3.7830000000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.96</v>
       </c>
@@ -1177,11 +1278,15 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <f>20*LOG10(C12/B12)</f>
+        <f t="shared" si="0"/>
         <v>5.6286887920120101</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
+        <v>3.8219999999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1195,11 +1300,15 @@
         <v>-8</v>
       </c>
       <c r="E13">
-        <f>20*LOG10(C13/B13)</f>
+        <f t="shared" si="0"/>
         <v>5.5708769503258821</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
+        <v>4.1399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2.1</v>
       </c>
@@ -1213,11 +1322,15 @@
         <v>-27</v>
       </c>
       <c r="E14">
-        <f t="shared" ref="E3:E40" si="0">20*LOG10(C14/B14)</f>
+        <f t="shared" ref="E14:E25" si="2">20*LOG10(C14/B14)</f>
         <v>4.5949046092478039</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
+        <v>3.8850000000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2.2000000000000002</v>
       </c>
@@ -1231,11 +1344,15 @@
         <v>-41</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3.2495179384456794</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="1">
+        <f t="shared" si="1"/>
+        <v>3.4540000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2.5</v>
       </c>
@@ -1249,11 +1366,15 @@
         <v>-62</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-0.85282127367623906</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1">
+        <f t="shared" si="1"/>
+        <v>2.4474999999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1267,11 +1388,15 @@
         <v>-74</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-5.1635499149342658</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1">
+        <f t="shared" si="1"/>
+        <v>1.788E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1285,11 +1410,15 @@
         <v>-84</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-12.754006951941923</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="1">
+        <f t="shared" si="1"/>
+        <v>2.2799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
@@ -1303,11 +1432,15 @@
         <v>-87</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-19.912703891950997</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1321,11 +1454,15 @@
         <v>-88</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-26.08223344858791</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="1">
+        <f t="shared" si="1"/>
+        <v>1.966E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>50</v>
       </c>
@@ -1339,11 +1476,15 @@
         <v>-89</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-34.067582464821477</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>100</v>
       </c>
@@ -1357,11 +1498,15 @@
         <v>-91</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-39.956242277036488</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9900000000000004E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>200</v>
       </c>
@@ -1375,11 +1520,15 @@
         <v>-93</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-45.846876329577775</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="1">
+        <f t="shared" si="1"/>
+        <v>2.0200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>500</v>
       </c>
@@ -1394,11 +1543,15 @@
         <v>-101</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-52.634167889600377</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="1">
+        <f t="shared" si="1"/>
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1000</v>
       </c>
@@ -1413,8 +1566,12 @@
         <v>-124</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-55.21554308628442</v>
+      </c>
+      <c r="F25" s="1">
+        <f>C25*A25*1000/10^6</f>
+        <v>3.4000000000000002E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1432,7 +1589,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1444,7 +1601,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ej1 casi terminado: conclusion y anexo
</commit_message>
<xml_diff>
--- a/Ej1/Mediciones/tc_tp3_ej1_hf.xlsx
+++ b/Ej1/Mediciones/tc_tp3_ej1_hf.xlsx
@@ -40,6 +40,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -69,9 +73,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -147,7 +157,7 @@
                 <c:pt idx="5">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="6" formatCode="0.0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
@@ -162,7 +172,7 @@
                 <c:pt idx="10">
                   <c:v>1.96</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="11" formatCode="0.00">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
@@ -174,10 +184,10 @@
                 <c:pt idx="14">
                   <c:v>2.5</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="15" formatCode="0.0">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="16" formatCode="0.0">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="17">
@@ -208,7 +218,7 @@
             <c:numRef>
               <c:f>Hoja1!$E$2:$E$40</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>-51.867476242857393</c:v>
@@ -327,7 +337,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -410,7 +420,7 @@
                 <c:pt idx="5">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="6" formatCode="0.0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
@@ -425,7 +435,7 @@
                 <c:pt idx="10">
                   <c:v>1.96</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="11" formatCode="0.00">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
@@ -437,10 +447,10 @@
                 <c:pt idx="14">
                   <c:v>2.5</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="15" formatCode="0.0">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="16" formatCode="0.0">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="17">
@@ -1015,13 +1025,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="A2:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1051,13 +1061,13 @@
       <c r="B2">
         <v>19.8</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>5.0500000000000003E-2</v>
       </c>
       <c r="D2">
         <v>89</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <f t="shared" ref="E2:E13" si="0">20*LOG10(C2/B2)</f>
         <v>-51.867476242857393</v>
       </c>
@@ -1073,18 +1083,18 @@
       <c r="B3">
         <v>19.8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>0.10100000000000001</v>
       </c>
       <c r="D3">
         <v>90</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <f t="shared" si="0"/>
         <v>-45.846876329577775</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F25" si="1">C3*A3*1000/10^6</f>
+        <f t="shared" ref="F3:F24" si="1">C3*A3*1000/10^6</f>
         <v>2.0200000000000001E-6</v>
       </c>
     </row>
@@ -1095,13 +1105,13 @@
       <c r="B4">
         <v>19.8</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>0.252</v>
       </c>
       <c r="D4">
         <v>89</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <f t="shared" si="0"/>
         <v>-37.905292989599737</v>
       </c>
@@ -1117,13 +1127,13 @@
       <c r="B5">
         <v>19.8</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0.5</v>
       </c>
       <c r="D5">
         <v>89</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <f t="shared" si="0"/>
         <v>-31.953903718510247</v>
       </c>
@@ -1139,13 +1149,13 @@
       <c r="B6">
         <v>19.8</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>1.01</v>
       </c>
       <c r="D6">
         <v>88</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>-25.846876329577771</v>
       </c>
@@ -1161,13 +1171,13 @@
       <c r="B7">
         <v>19.8</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>2.66</v>
       </c>
       <c r="D7">
         <v>86</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
         <v>-17.435671072609281</v>
       </c>
@@ -1177,19 +1187,19 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="5">
         <v>1</v>
       </c>
       <c r="B8">
         <v>19.8</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>6.68</v>
       </c>
       <c r="D8">
         <v>80</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>-9.4377745557197095</v>
       </c>
@@ -1205,13 +1215,13 @@
       <c r="B9">
         <v>10.8</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>8.9499999999999993</v>
       </c>
       <c r="D9">
         <v>65</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>-1.6320144034207558</v>
       </c>
@@ -1227,13 +1237,13 @@
       <c r="B10">
         <v>10.8</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>17.5</v>
       </c>
       <c r="D10">
         <v>34</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <f t="shared" si="0"/>
         <v>4.1922858639868945</v>
       </c>
@@ -1249,13 +1259,13 @@
       <c r="B11">
         <v>10.199999999999999</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>19.5</v>
       </c>
       <c r="D11">
         <v>5</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <f t="shared" si="0"/>
         <v>5.6286887920120101</v>
       </c>
@@ -1271,13 +1281,13 @@
       <c r="B12">
         <v>10.199999999999999</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>19.5</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
         <v>5.6286887920120101</v>
       </c>
@@ -1287,19 +1297,19 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="4">
         <v>2</v>
       </c>
       <c r="B13">
         <v>10.9</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>20.7</v>
       </c>
       <c r="D13">
         <v>-8</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <f t="shared" si="0"/>
         <v>5.5708769503258821</v>
       </c>
@@ -1315,13 +1325,13 @@
       <c r="B14">
         <v>10.9</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>18.5</v>
       </c>
       <c r="D14">
         <v>-27</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <f t="shared" ref="E14:E25" si="2">20*LOG10(C14/B14)</f>
         <v>4.5949046092478039</v>
       </c>
@@ -1337,13 +1347,13 @@
       <c r="B15">
         <v>10.8</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <v>15.7</v>
       </c>
       <c r="D15">
         <v>-41</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <f t="shared" si="2"/>
         <v>3.2495179384456794</v>
       </c>
@@ -1359,13 +1369,13 @@
       <c r="B16">
         <v>10.8</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>9.7899999999999991</v>
       </c>
       <c r="D16">
         <v>-62</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <f t="shared" si="2"/>
         <v>-0.85282127367623906</v>
       </c>
@@ -1375,19 +1385,19 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="5">
         <v>3</v>
       </c>
       <c r="B17">
         <v>10.8</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>5.96</v>
       </c>
       <c r="D17">
         <v>-74</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <f t="shared" si="2"/>
         <v>-5.1635499149342658</v>
       </c>
@@ -1397,19 +1407,19 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="5">
         <v>5</v>
       </c>
       <c r="B18">
         <v>19.8</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>4.5599999999999996</v>
       </c>
       <c r="D18">
         <v>-84</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <f t="shared" si="2"/>
         <v>-12.754006951941923</v>
       </c>
@@ -1425,13 +1435,13 @@
       <c r="B19">
         <v>19.8</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <v>2</v>
       </c>
       <c r="D19">
         <v>-87</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <f t="shared" si="2"/>
         <v>-19.912703891950997</v>
       </c>
@@ -1447,13 +1457,13 @@
       <c r="B20">
         <v>19.8</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>0.98299999999999998</v>
       </c>
       <c r="D20">
         <v>-88</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <f t="shared" si="2"/>
         <v>-26.08223344858791</v>
       </c>
@@ -1469,13 +1479,13 @@
       <c r="B21">
         <v>19.8</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>0.39200000000000002</v>
       </c>
       <c r="D21">
         <v>-89</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <f t="shared" si="2"/>
         <v>-34.067582464821477</v>
       </c>
@@ -1491,13 +1501,13 @@
       <c r="B22">
         <v>19.8</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <v>0.19900000000000001</v>
       </c>
       <c r="D22">
         <v>-91</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <f t="shared" si="2"/>
         <v>-39.956242277036488</v>
       </c>
@@ -1513,13 +1523,13 @@
       <c r="B23">
         <v>19.8</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>0.10100000000000001</v>
       </c>
       <c r="D23">
         <v>-93</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <f t="shared" si="2"/>
         <v>-45.846876329577775</v>
       </c>
@@ -1535,14 +1545,14 @@
       <c r="B24">
         <v>19.7</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="D24">
         <f>-360+259</f>
         <v>-101</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <f t="shared" si="2"/>
         <v>-52.634167889600377</v>
       </c>
@@ -1558,14 +1568,14 @@
       <c r="B25">
         <v>19.600000000000001</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="D25">
         <f>236-360</f>
         <v>-124</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <f t="shared" si="2"/>
         <v>-55.21554308628442</v>
       </c>

</xml_diff>